<commit_message>
Update orbital energy diagram example
</commit_message>
<xml_diff>
--- a/Examples/7 Orbital Energy Diagram.xlsx
+++ b/Examples/7 Orbital Energy Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_Program\Energy_Diagram_Plotter\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438BC937-710D-4443-90D4-D6C5AF546164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2809D2A8-0558-4760-AD89-62177B68BDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12222" xr2:uid="{F64FB10D-4E1D-44F9-B513-CD2FBC96F184}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
   <si>
     <t>B</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C8E728-1501-42E0-9757-586E386BB8A3}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -519,18 +519,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>1.1285622630755998</v>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>-5.7555808153518253</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>2.4097166080841657</v>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>-5.6868749538094594</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
@@ -538,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>-5.7555808153518253</v>
+        <v>-5.5622750179649882</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>-5.6868749538094594</v>
+        <v>-5.3981975915602733</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>-5.5622750179649882</v>
+        <v>-5.0047683347877756</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>-5.3981975915602733</v>
+        <v>-1.4357864627864572</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>-5.0047683347877756</v>
+        <v>-8.3240332354341029E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>-1.4357864627864572</v>
+        <v>0.24461081814580726</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>-8.3240332354341029E-2</v>
+        <v>0.44651913181523756</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.24461081814580726</v>
+        <v>0.49782685687908984</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
@@ -602,58 +602,26 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0.44651913181523756</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0.49782685687908984</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
         <v>0.55214206394723164</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1.3705312948177686</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>2.4245406670088436</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B33" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B34" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="C45" t="s">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="C46" t="s">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C40" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>